<commit_message>
Day 6 in Pascal, day1 cleanup
</commit_message>
<xml_diff>
--- a/Day1.xlsx
+++ b/Day1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\AOC-2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\AOC-2025\AdventOfCode2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0632AC30-0F97-462F-9314-E21151B8EBE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF3768A-314F-4E85-9B04-9F45EAA005E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16371" yWindow="0" windowWidth="16629" windowHeight="17880" xr2:uid="{298A57D0-EFE6-45FE-9F90-F564587C39B3}"/>
+    <workbookView xWindow="609" yWindow="369" windowWidth="27128" windowHeight="16337" xr2:uid="{298A57D0-EFE6-45FE-9F90-F564587C39B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>L68</t>
   </si>
@@ -85,12 +85,18 @@
   <si>
     <t>Tot</t>
   </si>
+  <si>
+    <t>Part1</t>
+  </si>
+  <si>
+    <t>Part 2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,6 +108,14 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -124,11 +138,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D724C5B2-EDAF-4718-8864-271865443BB0}">
   <dimension ref="A2:M4667"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6"/>
@@ -1030,6 +1045,16 @@
       </c>
     </row>
     <row r="13" spans="1:13">
+      <c r="G13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13">
+        <f>SUM(H3:H12)</f>
+        <v>3</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="M13">
         <f>SUM(M3:M12)</f>
         <v>6</v>
@@ -14985,7 +15010,7 @@
     <row r="4667" spans="1:13">
       <c r="H4667">
         <f>SUM(H3:H4666)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M4667">
         <f>SUM(M3:M4666)</f>

</xml_diff>